<commit_message>
Updated station lists and wrote a small helper script.
</commit_message>
<xml_diff>
--- a/Test/Data/crocus_stations.xlsx
+++ b/Test/Data/crocus_stations.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="106">
   <si>
     <t>ARNØYA</t>
   </si>
@@ -32,6 +32,9 @@
     <t>BJORLI</t>
   </si>
   <si>
+    <t>BUSNES</t>
+  </si>
+  <si>
     <t>DIVIDALEN</t>
   </si>
   <si>
@@ -62,6 +65,9 @@
     <t>FOLGEFONNA</t>
   </si>
   <si>
+    <t>FOLGEFONNA SKISENTER</t>
+  </si>
+  <si>
     <t>FOLGEFONNA SKISENTER TOPP</t>
   </si>
   <si>
@@ -71,6 +77,9 @@
     <t>FOLLDAL - FREDHEIM</t>
   </si>
   <si>
+    <t>FRØYSTUL</t>
+  </si>
+  <si>
     <t>GAUSTATOPPEN</t>
   </si>
   <si>
@@ -83,9 +92,15 @@
     <t>GLOMFJORD</t>
   </si>
   <si>
+    <t>GLOMFJORD - SKIHYTTA</t>
+  </si>
+  <si>
     <t>GLOMFJORD - TVERRFJELLET</t>
   </si>
   <si>
+    <t>GROSET</t>
+  </si>
+  <si>
     <t>GROTLI</t>
   </si>
   <si>
@@ -98,6 +113,15 @@
     <t>GULSVIK II</t>
   </si>
   <si>
+    <t>HANSBU</t>
+  </si>
+  <si>
+    <t>HAUKELISETER</t>
+  </si>
+  <si>
+    <t>HAUKELISETER TESTFELT</t>
+  </si>
+  <si>
     <t>HEMSEDAL</t>
   </si>
   <si>
@@ -131,12 +155,21 @@
     <t>JORDALEN - NÅSEN</t>
   </si>
   <si>
+    <t>JOSTEDALEN</t>
+  </si>
+  <si>
+    <t>JOSTEDALEN - BREHEIMSENTERET</t>
+  </si>
+  <si>
     <t>JUVVASSHØE</t>
   </si>
   <si>
     <t>KISTEFJELL</t>
   </si>
   <si>
+    <t>KLEVAVATNET</t>
+  </si>
+  <si>
     <t>LEBERGSFJELLET</t>
   </si>
   <si>
@@ -155,12 +188,24 @@
     <t>LYNGEN - GJERDVASSBU</t>
   </si>
   <si>
+    <t>MALANGEN</t>
+  </si>
+  <si>
+    <t>MALANGEN - PÅLFINNMOEN</t>
+  </si>
+  <si>
     <t>MANNEN</t>
   </si>
   <si>
     <t>MIDTSTOVA</t>
   </si>
   <si>
+    <t>MOGEN</t>
+  </si>
+  <si>
+    <t>MOGEN TEST</t>
+  </si>
+  <si>
     <t>MOH</t>
   </si>
   <si>
@@ -188,6 +233,9 @@
     <t>NORDNESFJELLET</t>
   </si>
   <si>
+    <t>NUVSVÅG</t>
+  </si>
+  <si>
     <t>OPPDAL</t>
   </si>
   <si>
@@ -221,15 +269,27 @@
     <t>STRAUMSNES</t>
   </si>
   <si>
+    <t>STRENGEN</t>
+  </si>
+  <si>
     <t>StasjonsID</t>
   </si>
   <si>
+    <t>SÆTERTINDEN</t>
+  </si>
+  <si>
+    <t>SÆTERTINDEN VED TJELDSUNDET</t>
+  </si>
+  <si>
     <t>SØLENDET</t>
   </si>
   <si>
     <t>TAMOKDALEN</t>
   </si>
   <si>
+    <t>TINNOSDAMMEN</t>
+  </si>
+  <si>
     <t>TROMSØ</t>
   </si>
   <si>
@@ -267,6 +327,12 @@
   </si>
   <si>
     <t>ØKSFJORD - DEALLJA</t>
+  </si>
+  <si>
+    <t>ØRSTA</t>
+  </si>
+  <si>
+    <t>ØRSTA - EITREFJELL</t>
   </si>
 </sst>
 </file>
@@ -598,375 +664,375 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <outlinePr summaryRight="1" summaryBelow="1"/>
   </sheetPr>
-  <dimension ref="A1:I52"/>
+  <dimension ref="A1:I68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection sqref="A1" activeCell="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col width="9.10" max="1" min="1"/>
-    <col width="9.10" max="2" min="2"/>
-    <col width="9.10" max="3" min="3"/>
-    <col width="9.10" max="4" min="4"/>
-    <col width="9.10" max="5" min="5"/>
-    <col width="9.10" max="6" min="6"/>
-    <col width="9.10" max="7" min="7"/>
-    <col width="9.10" max="8" min="8"/>
-    <col width="9.10" max="9" min="9"/>
+    <col max="1" min="1" width="9.10"/>
+    <col max="2" min="2" width="9.10"/>
+    <col max="3" min="3" width="9.10"/>
+    <col max="4" min="4" width="9.10"/>
+    <col max="5" min="5" width="9.10"/>
+    <col max="6" min="6" width="9.10"/>
+    <col max="7" min="7" width="9.10"/>
+    <col max="8" min="8" width="9.10"/>
+    <col max="9" min="9" width="9.10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>68</v>
+        <v>85</v>
       </c>
       <c r="B1" t="s">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="C1" t="s">
-        <v>79</v>
+        <v>99</v>
       </c>
       <c r="D1" t="s">
-        <v>77</v>
+        <v>97</v>
       </c>
       <c r="E1" t="s">
-        <v>78</v>
+        <v>98</v>
       </c>
       <c r="F1" t="s">
-        <v>74</v>
+        <v>94</v>
       </c>
       <c r="G1" t="s">
-        <v>75</v>
+        <v>95</v>
       </c>
       <c r="H1" t="s">
-        <v>73</v>
+        <v>93</v>
       </c>
       <c r="I1" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="n">
-        <v>15890</v>
+        <v>61630</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="D2" t="n">
-        <v>62.0162</v>
+        <v>62.2583</v>
       </c>
       <c r="E2" t="n">
-        <v>7.6637</v>
+        <v>8.2</v>
       </c>
       <c r="F2" t="n">
-        <v>116537</v>
+        <v>147324</v>
       </c>
       <c r="G2" t="n">
-        <v>6897707</v>
+        <v>6921509</v>
       </c>
       <c r="H2" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="I2" t="n">
-        <v>872</v>
+        <v>579</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="n">
-        <v>89985</v>
+        <v>80707</v>
       </c>
       <c r="B3" t="s">
-        <v>64</v>
+        <v>24</v>
       </c>
       <c r="C3" t="s">
-        <v>64</v>
+        <v>26</v>
       </c>
       <c r="D3" t="n">
-        <v>69.1025</v>
+        <v>66.8338</v>
       </c>
       <c r="E3" t="n">
-        <v>19.5442</v>
+        <v>13.9117</v>
       </c>
       <c r="F3" t="n">
-        <v>680754</v>
+        <v>452226</v>
       </c>
       <c r="G3" t="n">
-        <v>7672492</v>
+        <v>7413270</v>
       </c>
       <c r="H3" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="I3" t="n">
-        <v>1020</v>
+        <v>930</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="n">
-        <v>23550</v>
+        <v>15270</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
+        <v>48</v>
       </c>
       <c r="D4" t="n">
-        <v>61.2508</v>
+        <v>61.6775</v>
       </c>
       <c r="E4" t="n">
-        <v>8.9228</v>
+        <v>8.369</v>
       </c>
       <c r="F4" t="n">
-        <v>174233</v>
+        <v>149452</v>
       </c>
       <c r="G4" t="n">
-        <v>6805891</v>
+        <v>6856140</v>
       </c>
       <c r="H4" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="I4" t="n">
-        <v>965</v>
+        <v>1894</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="n">
-        <v>89980</v>
+        <v>55420</v>
       </c>
       <c r="B5" t="s">
-        <v>70</v>
+        <v>46</v>
       </c>
       <c r="C5" t="s">
-        <v>70</v>
+        <v>47</v>
       </c>
       <c r="D5" t="n">
-        <v>69.0935</v>
+        <v>61.6517</v>
       </c>
       <c r="E5" t="n">
-        <v>19.6278</v>
+        <v>7.2765</v>
       </c>
       <c r="F5" t="n">
-        <v>684149</v>
+        <v>91536</v>
       </c>
       <c r="G5" t="n">
-        <v>7671740</v>
+        <v>6859663</v>
       </c>
       <c r="H5" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="I5" t="n">
-        <v>230</v>
+        <v>243</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="n">
-        <v>89940</v>
+        <v>91500</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>71</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
+        <v>71</v>
       </c>
       <c r="D6" t="n">
-        <v>68.7817</v>
+        <v>69.5738</v>
       </c>
       <c r="E6" t="n">
-        <v>19.7017</v>
+        <v>20.4253</v>
       </c>
       <c r="F6" t="n">
-        <v>689747</v>
+        <v>711075</v>
       </c>
       <c r="G6" t="n">
-        <v>7637284</v>
+        <v>7727719</v>
       </c>
       <c r="H6" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="I6" t="n">
-        <v>204</v>
+        <v>700</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="n">
-        <v>84500</v>
+        <v>51990</v>
       </c>
       <c r="B7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D7" t="n">
-        <v>68.432</v>
+        <v>60.8655</v>
       </c>
       <c r="E7" t="n">
-        <v>17.662</v>
+        <v>6.4733</v>
       </c>
       <c r="F7" t="n">
-        <v>609178</v>
+        <v>37781</v>
       </c>
       <c r="G7" t="n">
-        <v>7593389</v>
+        <v>6777930</v>
       </c>
       <c r="H7" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="I7" t="n">
-        <v>200</v>
+        <v>700</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="n">
-        <v>53160</v>
+        <v>53480</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="C8" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="D8" t="n">
-        <v>60.9004</v>
+        <v>60.7192</v>
       </c>
       <c r="E8" t="n">
-        <v>6.7243</v>
+        <v>7.2085</v>
       </c>
       <c r="F8" t="n">
-        <v>51827</v>
+        <v>75561</v>
       </c>
       <c r="G8" t="n">
-        <v>6780047</v>
+        <v>6756741</v>
       </c>
       <c r="H8" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="I8" t="n">
-        <v>614</v>
+        <v>960</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="n">
-        <v>40880</v>
+        <v>15890</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C9" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D9" t="n">
-        <v>59.5766</v>
+        <v>62.0162</v>
       </c>
       <c r="E9" t="n">
-        <v>7.3897</v>
+        <v>7.6637</v>
       </c>
       <c r="F9" t="n">
-        <v>70721</v>
+        <v>116537</v>
       </c>
       <c r="G9" t="n">
-        <v>6628898</v>
+        <v>6897707</v>
       </c>
       <c r="H9" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="I9" t="n">
-        <v>841</v>
+        <v>872</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="n">
-        <v>13655</v>
+        <v>31520</v>
       </c>
       <c r="B10" t="s">
-        <v>65</v>
+        <v>27</v>
       </c>
       <c r="C10" t="s">
-        <v>65</v>
+        <v>27</v>
       </c>
       <c r="D10" t="n">
-        <v>61.5308</v>
+        <v>59.8358</v>
       </c>
       <c r="E10" t="n">
-        <v>9.4023</v>
+        <v>8.315</v>
       </c>
       <c r="F10" t="n">
-        <v>202568</v>
+        <v>125702</v>
       </c>
       <c r="G10" t="n">
-        <v>6834700</v>
+        <v>6652036</v>
       </c>
       <c r="H10" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="I10" t="n">
-        <v>928</v>
+        <v>949</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="n">
-        <v>51980</v>
+        <v>84500</v>
       </c>
       <c r="B11" t="s">
-        <v>50</v>
+        <v>83</v>
       </c>
       <c r="C11" t="s">
-        <v>50</v>
+        <v>83</v>
       </c>
       <c r="D11" t="n">
-        <v>60.8603</v>
+        <v>68.432</v>
       </c>
       <c r="E11" t="n">
-        <v>6.4675</v>
+        <v>17.662</v>
       </c>
       <c r="F11" t="n">
-        <v>37392</v>
+        <v>609178</v>
       </c>
       <c r="G11" t="n">
-        <v>6777396</v>
+        <v>7593389</v>
       </c>
       <c r="H11" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="I11" t="n">
-        <v>853</v>
+        <v>200</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="n">
-        <v>91120</v>
+        <v>91130</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="C12" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="D12" t="n">
-        <v>69.5592</v>
+        <v>69.5588</v>
       </c>
       <c r="E12" t="n">
-        <v>20.1502</v>
+        <v>20.094</v>
       </c>
       <c r="F12" t="n">
-        <v>700531</v>
+        <v>698351</v>
       </c>
       <c r="G12" t="n">
-        <v>7725170</v>
+        <v>7724942</v>
       </c>
       <c r="H12" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="I12" t="n">
-        <v>670</v>
+        <v>710</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -974,10 +1040,10 @@
         <v>14200</v>
       </c>
       <c r="B13" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="C13" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="D13" t="n">
         <v>61.7247</v>
@@ -992,7 +1058,7 @@
         <v>6857396</v>
       </c>
       <c r="H13" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="I13" t="n">
         <v>599</v>
@@ -1003,10 +1069,10 @@
         <v>9160</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C14" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D14" t="n">
         <v>62.1282</v>
@@ -1021,7 +1087,7 @@
         <v>6898544</v>
       </c>
       <c r="H14" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="I14" t="n">
         <v>694</v>
@@ -1032,10 +1098,10 @@
         <v>49087</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C15" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D15" t="n">
         <v>60.2178</v>
@@ -1050,7 +1116,7 @@
         <v>6706520</v>
       </c>
       <c r="H15" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="I15" t="n">
         <v>1390</v>
@@ -1058,118 +1124,118 @@
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="n">
-        <v>25110</v>
+        <v>64700</v>
       </c>
       <c r="B16" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="C16" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="D16" t="n">
-        <v>60.8548</v>
+        <v>62.722</v>
       </c>
       <c r="E16" t="n">
-        <v>8.593</v>
+        <v>8.7753</v>
       </c>
       <c r="F16" t="n">
-        <v>152274</v>
+        <v>182072</v>
       </c>
       <c r="G16" t="n">
-        <v>6763621</v>
+        <v>6969987</v>
       </c>
       <c r="H16" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="I16" t="n">
-        <v>604</v>
+        <v>405</v>
       </c>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" t="n">
-        <v>89010</v>
+        <v>23550</v>
       </c>
       <c r="B17" t="s">
-        <v>39</v>
+        <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>39</v>
+        <v>3</v>
       </c>
       <c r="D17" t="n">
-        <v>69.2897</v>
+        <v>61.2508</v>
       </c>
       <c r="E17" t="n">
-        <v>18.1288</v>
+        <v>8.9228</v>
       </c>
       <c r="F17" t="n">
-        <v>623439</v>
+        <v>174233</v>
       </c>
       <c r="G17" t="n">
-        <v>7689819</v>
+        <v>6805891</v>
       </c>
       <c r="H17" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="I17" t="n">
-        <v>982</v>
+        <v>965</v>
       </c>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" t="n">
-        <v>9380</v>
+        <v>10800</v>
       </c>
       <c r="B18" t="s">
-        <v>66</v>
+        <v>88</v>
       </c>
       <c r="C18" t="s">
-        <v>66</v>
+        <v>88</v>
       </c>
       <c r="D18" t="n">
-        <v>62.2958</v>
+        <v>62.6794</v>
       </c>
       <c r="E18" t="n">
-        <v>9.352</v>
+        <v>11.8153</v>
       </c>
       <c r="F18" t="n">
-        <v>207315</v>
+        <v>336969</v>
       </c>
       <c r="G18" t="n">
-        <v>6919920</v>
+        <v>6953897</v>
       </c>
       <c r="H18" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="I18" t="n">
-        <v>1475</v>
+        <v>760</v>
       </c>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" t="n">
-        <v>63820</v>
+        <v>92650</v>
       </c>
       <c r="B19" t="s">
-        <v>8</v>
+        <v>72</v>
       </c>
       <c r="C19" t="s">
-        <v>8</v>
+        <v>72</v>
       </c>
       <c r="D19" t="n">
-        <v>62.4473</v>
+        <v>70.2368</v>
       </c>
       <c r="E19" t="n">
-        <v>9.5827</v>
+        <v>22.0705</v>
       </c>
       <c r="F19" t="n">
-        <v>220664</v>
+        <v>766303</v>
       </c>
       <c r="G19" t="n">
-        <v>6935732</v>
+        <v>7807768</v>
       </c>
       <c r="H19" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="I19" t="n">
-        <v>680</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -1177,10 +1243,10 @@
         <v>84210</v>
       </c>
       <c r="B20" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="C20" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="D20" t="n">
         <v>68.1905</v>
@@ -1195,7 +1261,7 @@
         <v>7566719</v>
       </c>
       <c r="H20" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="I20" t="n">
         <v>740</v>
@@ -1203,28 +1269,28 @@
     </row>
     <row r="21" spans="1:9">
       <c r="A21" t="n">
-        <v>42940</v>
+        <v>92860</v>
       </c>
       <c r="B21" t="s">
-        <v>62</v>
+        <v>102</v>
       </c>
       <c r="C21" t="s">
-        <v>63</v>
+        <v>103</v>
       </c>
       <c r="D21" t="n">
-        <v>58.923</v>
+        <v>70.1728</v>
       </c>
       <c r="E21" t="n">
-        <v>6.9097</v>
+        <v>22.3413</v>
       </c>
       <c r="F21" t="n">
-        <v>34883</v>
+        <v>777319</v>
       </c>
       <c r="G21" t="n">
-        <v>6559675</v>
+        <v>7801885</v>
       </c>
       <c r="H21" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="I21" t="n">
         <v>560</v>
@@ -1232,703 +1298,703 @@
     </row>
     <row r="22" spans="1:9">
       <c r="A22" t="n">
-        <v>60240</v>
+        <v>9310</v>
       </c>
       <c r="B22" t="s">
-        <v>81</v>
+        <v>37</v>
       </c>
       <c r="C22" t="s">
-        <v>81</v>
+        <v>38</v>
       </c>
       <c r="D22" t="n">
-        <v>62.191</v>
+        <v>62.2207</v>
       </c>
       <c r="E22" t="n">
-        <v>6.9933</v>
+        <v>9.5423</v>
       </c>
       <c r="F22" t="n">
-        <v>84027</v>
+        <v>216453</v>
       </c>
       <c r="G22" t="n">
-        <v>6921226</v>
+        <v>6910728</v>
       </c>
       <c r="H22" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="I22" t="n">
-        <v>900</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" t="n">
-        <v>46432</v>
+        <v>16400</v>
       </c>
       <c r="B23" t="s">
-        <v>60</v>
+        <v>8</v>
       </c>
       <c r="C23" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="D23" t="n">
-        <v>59.8357</v>
+        <v>62.0172</v>
       </c>
       <c r="E23" t="n">
-        <v>6.7108</v>
+        <v>9.2143</v>
       </c>
       <c r="F23" t="n">
-        <v>36163</v>
+        <v>197420</v>
       </c>
       <c r="G23" t="n">
-        <v>6662199</v>
+        <v>6889604</v>
       </c>
       <c r="H23" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="I23" t="n">
-        <v>1370</v>
+        <v>560</v>
       </c>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" t="n">
-        <v>46430</v>
+        <v>30810</v>
       </c>
       <c r="B24" t="s">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="C24" t="s">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="D24" t="n">
-        <v>59.8315</v>
+        <v>59.7238</v>
       </c>
       <c r="E24" t="n">
-        <v>6.733</v>
+        <v>9.0245</v>
       </c>
       <c r="F24" t="n">
-        <v>37342</v>
+        <v>164226</v>
       </c>
       <c r="G24" t="n">
-        <v>6661578</v>
+        <v>6635794</v>
       </c>
       <c r="H24" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="I24" t="n">
-        <v>1010</v>
+        <v>191</v>
       </c>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" t="n">
-        <v>24710</v>
+        <v>33950</v>
       </c>
       <c r="B25" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="C25" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="D25" t="n">
-        <v>60.383</v>
+        <v>59.8118</v>
       </c>
       <c r="E25" t="n">
-        <v>9.605</v>
+        <v>7.2143</v>
       </c>
       <c r="F25" t="n">
-        <v>202790</v>
+        <v>63934</v>
       </c>
       <c r="G25" t="n">
-        <v>6706244</v>
+        <v>6656121</v>
       </c>
       <c r="H25" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="I25" t="n">
-        <v>142</v>
+        <v>990</v>
       </c>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" t="n">
-        <v>91500</v>
+        <v>46430</v>
       </c>
       <c r="B26" t="s">
-        <v>56</v>
+        <v>76</v>
       </c>
       <c r="C26" t="s">
-        <v>56</v>
+        <v>76</v>
       </c>
       <c r="D26" t="n">
-        <v>69.5738</v>
+        <v>59.8315</v>
       </c>
       <c r="E26" t="n">
-        <v>20.4253</v>
+        <v>6.733</v>
       </c>
       <c r="F26" t="n">
-        <v>711075</v>
+        <v>37342</v>
       </c>
       <c r="G26" t="n">
-        <v>7727719</v>
+        <v>6661578</v>
       </c>
       <c r="H26" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="I26" t="n">
-        <v>700</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="27" spans="1:9">
       <c r="A27" t="n">
-        <v>91130</v>
+        <v>49800</v>
       </c>
       <c r="B27" t="s">
-        <v>43</v>
+        <v>10</v>
       </c>
       <c r="C27" t="s">
-        <v>45</v>
+        <v>11</v>
       </c>
       <c r="D27" t="n">
-        <v>69.5588</v>
+        <v>60.4085</v>
       </c>
       <c r="E27" t="n">
-        <v>20.094</v>
+        <v>7.2798</v>
       </c>
       <c r="F27" t="n">
-        <v>698351</v>
+        <v>75367</v>
       </c>
       <c r="G27" t="n">
-        <v>7724942</v>
+        <v>6721839</v>
       </c>
       <c r="H27" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="I27" t="n">
-        <v>710</v>
+        <v>735</v>
       </c>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" t="n">
-        <v>25630</v>
+        <v>51980</v>
       </c>
       <c r="B28" t="s">
-        <v>19</v>
+        <v>65</v>
       </c>
       <c r="C28" t="s">
-        <v>20</v>
+        <v>65</v>
       </c>
       <c r="D28" t="n">
-        <v>60.53</v>
+        <v>60.8603</v>
       </c>
       <c r="E28" t="n">
-        <v>8.1948</v>
+        <v>6.4675</v>
       </c>
       <c r="F28" t="n">
-        <v>126964</v>
+        <v>37392</v>
       </c>
       <c r="G28" t="n">
-        <v>6729759</v>
+        <v>6777396</v>
       </c>
       <c r="H28" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="I28" t="n">
-        <v>772</v>
+        <v>853</v>
       </c>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" t="n">
-        <v>32890</v>
+        <v>25110</v>
       </c>
       <c r="B29" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C29" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D29" t="n">
-        <v>59.497</v>
+        <v>60.8548</v>
       </c>
       <c r="E29" t="n">
-        <v>8.1992</v>
+        <v>8.593</v>
       </c>
       <c r="F29" t="n">
-        <v>115363</v>
+        <v>152274</v>
       </c>
       <c r="G29" t="n">
-        <v>6615099</v>
+        <v>6763621</v>
       </c>
       <c r="H29" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="I29" t="n">
-        <v>560</v>
+        <v>604</v>
       </c>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" t="n">
-        <v>63705</v>
+        <v>60190</v>
       </c>
       <c r="B30" t="s">
-        <v>57</v>
+        <v>75</v>
       </c>
       <c r="C30" t="s">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="D30" t="n">
-        <v>62.6043</v>
+        <v>62.3065</v>
       </c>
       <c r="E30" t="n">
-        <v>9.6667</v>
+        <v>6.849</v>
       </c>
       <c r="F30" t="n">
-        <v>226433</v>
+        <v>78180</v>
       </c>
       <c r="G30" t="n">
-        <v>6952819</v>
+        <v>6934957</v>
       </c>
       <c r="H30" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="I30" t="n">
-        <v>604</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="31" spans="1:9">
       <c r="A31" t="n">
-        <v>57790</v>
+        <v>60810</v>
       </c>
       <c r="B31" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C31" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D31" t="n">
-        <v>61.6788</v>
+        <v>62.5158</v>
       </c>
       <c r="E31" t="n">
-        <v>5.2007</v>
+        <v>6.8717</v>
       </c>
       <c r="F31" t="n">
-        <v>-17258</v>
+        <v>82285</v>
       </c>
       <c r="G31" t="n">
-        <v>6877476</v>
+        <v>6957992</v>
       </c>
       <c r="H31" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="I31" t="n">
-        <v>715</v>
+        <v>625</v>
       </c>
     </row>
     <row r="32" spans="1:9">
       <c r="A32" t="n">
-        <v>84630</v>
+        <v>63705</v>
       </c>
       <c r="B32" t="s">
-        <v>54</v>
+        <v>73</v>
       </c>
       <c r="C32" t="s">
-        <v>55</v>
+        <v>74</v>
       </c>
       <c r="D32" t="n">
-        <v>68.421</v>
+        <v>62.6043</v>
       </c>
       <c r="E32" t="n">
-        <v>17.4802</v>
+        <v>9.6667</v>
       </c>
       <c r="F32" t="n">
-        <v>601774</v>
+        <v>226433</v>
       </c>
       <c r="G32" t="n">
-        <v>7591852</v>
+        <v>6952819</v>
       </c>
       <c r="H32" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="I32" t="n">
-        <v>1000</v>
+        <v>604</v>
       </c>
     </row>
     <row r="33" spans="1:9">
       <c r="A33" t="n">
-        <v>91729</v>
+        <v>63820</v>
       </c>
       <c r="B33" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C33" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D33" t="n">
-        <v>70.075</v>
+        <v>62.4473</v>
       </c>
       <c r="E33" t="n">
-        <v>20.431</v>
+        <v>9.5827</v>
       </c>
       <c r="F33" t="n">
-        <v>706325</v>
+        <v>220664</v>
       </c>
       <c r="G33" t="n">
-        <v>7783439</v>
+        <v>6935732</v>
       </c>
       <c r="H33" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="I33" t="n">
-        <v>850</v>
+        <v>680</v>
       </c>
     </row>
     <row r="34" spans="1:9">
       <c r="A34" t="n">
-        <v>54710</v>
+        <v>90100</v>
       </c>
       <c r="B34" t="s">
-        <v>11</v>
+        <v>57</v>
       </c>
       <c r="C34" t="s">
-        <v>12</v>
+        <v>58</v>
       </c>
       <c r="D34" t="n">
-        <v>61.178</v>
+        <v>69.414</v>
       </c>
       <c r="E34" t="n">
-        <v>8.1125</v>
+        <v>18.6773</v>
       </c>
       <c r="F34" t="n">
-        <v>130049</v>
+        <v>644226</v>
       </c>
       <c r="G34" t="n">
-        <v>6802130</v>
+        <v>7704861</v>
       </c>
       <c r="H34" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="I34" t="n">
-        <v>956</v>
+        <v>124</v>
       </c>
     </row>
     <row r="35" spans="1:9">
       <c r="A35" t="n">
-        <v>15270</v>
+        <v>49085</v>
       </c>
       <c r="B35" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="C35" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="D35" t="n">
-        <v>61.6775</v>
+        <v>60.2263</v>
       </c>
       <c r="E35" t="n">
-        <v>8.369</v>
+        <v>6.4347</v>
       </c>
       <c r="F35" t="n">
-        <v>149452</v>
+        <v>26414</v>
       </c>
       <c r="G35" t="n">
-        <v>6856140</v>
+        <v>6707426</v>
       </c>
       <c r="H35" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="I35" t="n">
-        <v>1894</v>
+        <v>1212</v>
       </c>
     </row>
     <row r="36" spans="1:9">
       <c r="A36" t="n">
-        <v>92860</v>
+        <v>84630</v>
       </c>
       <c r="B36" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="C36" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="D36" t="n">
-        <v>70.1728</v>
+        <v>68.421</v>
       </c>
       <c r="E36" t="n">
-        <v>22.3413</v>
+        <v>17.4802</v>
       </c>
       <c r="F36" t="n">
-        <v>777319</v>
+        <v>601774</v>
       </c>
       <c r="G36" t="n">
-        <v>7801885</v>
+        <v>7591852</v>
       </c>
       <c r="H36" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="I36" t="n">
-        <v>560</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="37" spans="1:9">
       <c r="A37" t="n">
-        <v>51990</v>
+        <v>31661</v>
       </c>
       <c r="B37" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="C37" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="D37" t="n">
-        <v>60.8655</v>
+        <v>60.02</v>
       </c>
       <c r="E37" t="n">
-        <v>6.4733</v>
+        <v>7.91</v>
       </c>
       <c r="F37" t="n">
-        <v>37781</v>
+        <v>105281</v>
       </c>
       <c r="G37" t="n">
-        <v>6777930</v>
+        <v>6674833</v>
       </c>
       <c r="H37" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="I37" t="n">
-        <v>700</v>
+        <v>954</v>
       </c>
     </row>
     <row r="38" spans="1:9">
       <c r="A38" t="n">
-        <v>16400</v>
+        <v>25830</v>
       </c>
       <c r="B38" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C38" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D38" t="n">
-        <v>62.0172</v>
+        <v>60.5917</v>
       </c>
       <c r="E38" t="n">
-        <v>9.2143</v>
+        <v>7.5242</v>
       </c>
       <c r="F38" t="n">
-        <v>197420</v>
+        <v>91089</v>
       </c>
       <c r="G38" t="n">
-        <v>6889604</v>
+        <v>6740599</v>
       </c>
       <c r="H38" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="I38" t="n">
-        <v>560</v>
+        <v>1210</v>
       </c>
     </row>
     <row r="39" spans="1:9">
       <c r="A39" t="n">
-        <v>60810</v>
+        <v>24710</v>
       </c>
       <c r="B39" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C39" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="D39" t="n">
-        <v>62.5158</v>
+        <v>60.383</v>
       </c>
       <c r="E39" t="n">
-        <v>6.8717</v>
+        <v>9.605</v>
       </c>
       <c r="F39" t="n">
-        <v>82285</v>
+        <v>202790</v>
       </c>
       <c r="G39" t="n">
-        <v>6957992</v>
+        <v>6706244</v>
       </c>
       <c r="H39" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="I39" t="n">
-        <v>625</v>
+        <v>142</v>
       </c>
     </row>
     <row r="40" spans="1:9">
       <c r="A40" t="n">
-        <v>80707</v>
+        <v>57790</v>
       </c>
       <c r="B40" t="s">
-        <v>21</v>
+        <v>64</v>
       </c>
       <c r="C40" t="s">
-        <v>22</v>
+        <v>64</v>
       </c>
       <c r="D40" t="n">
-        <v>66.8338</v>
+        <v>61.6788</v>
       </c>
       <c r="E40" t="n">
-        <v>13.9117</v>
+        <v>5.2007</v>
       </c>
       <c r="F40" t="n">
-        <v>452226</v>
+        <v>-17258</v>
       </c>
       <c r="G40" t="n">
-        <v>7413270</v>
+        <v>6877476</v>
       </c>
       <c r="H40" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="I40" t="n">
-        <v>930</v>
+        <v>715</v>
       </c>
     </row>
     <row r="41" spans="1:9">
       <c r="A41" t="n">
-        <v>9310</v>
+        <v>89010</v>
       </c>
       <c r="B41" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="C41" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="D41" t="n">
-        <v>62.2207</v>
+        <v>69.2897</v>
       </c>
       <c r="E41" t="n">
-        <v>9.5423</v>
+        <v>18.1288</v>
       </c>
       <c r="F41" t="n">
-        <v>216453</v>
+        <v>623439</v>
       </c>
       <c r="G41" t="n">
-        <v>6910728</v>
+        <v>7689819</v>
       </c>
       <c r="H41" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="I41" t="n">
-        <v>1012</v>
+        <v>982</v>
       </c>
     </row>
     <row r="42" spans="1:9">
       <c r="A42" t="n">
-        <v>90400</v>
+        <v>31500</v>
       </c>
       <c r="B42" t="s">
-        <v>71</v>
+        <v>20</v>
       </c>
       <c r="C42" t="s">
-        <v>72</v>
+        <v>20</v>
       </c>
       <c r="D42" t="n">
-        <v>69.6523</v>
+        <v>59.8247</v>
       </c>
       <c r="E42" t="n">
-        <v>18.9057</v>
+        <v>8.3477</v>
       </c>
       <c r="F42" t="n">
-        <v>651477</v>
+        <v>127405</v>
       </c>
       <c r="G42" t="n">
-        <v>7731942</v>
+        <v>6650619</v>
       </c>
       <c r="H42" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="I42" t="n">
-        <v>20</v>
+        <v>875</v>
       </c>
     </row>
     <row r="43" spans="1:9">
       <c r="A43" t="n">
-        <v>31970</v>
+        <v>46432</v>
       </c>
       <c r="B43" t="s">
-        <v>18</v>
+        <v>76</v>
       </c>
       <c r="C43" t="s">
-        <v>18</v>
+        <v>77</v>
       </c>
       <c r="D43" t="n">
-        <v>59.8497</v>
+        <v>59.8357</v>
       </c>
       <c r="E43" t="n">
-        <v>8.6562</v>
+        <v>6.7108</v>
       </c>
       <c r="F43" t="n">
-        <v>144914</v>
+        <v>36163</v>
       </c>
       <c r="G43" t="n">
-        <v>6651697</v>
+        <v>6662199</v>
       </c>
       <c r="H43" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="I43" t="n">
-        <v>1804</v>
+        <v>1370</v>
       </c>
     </row>
     <row r="44" spans="1:9">
       <c r="A44" t="n">
-        <v>49800</v>
+        <v>31680</v>
       </c>
       <c r="B44" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="C44" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="D44" t="n">
-        <v>60.4085</v>
+        <v>60.0825</v>
       </c>
       <c r="E44" t="n">
-        <v>7.2798</v>
+        <v>7.4247</v>
       </c>
       <c r="F44" t="n">
-        <v>75367</v>
+        <v>79139</v>
       </c>
       <c r="G44" t="n">
-        <v>6721839</v>
+        <v>6684766</v>
       </c>
       <c r="H44" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="I44" t="n">
-        <v>735</v>
+        <v>1260</v>
       </c>
     </row>
     <row r="45" spans="1:9">
       <c r="A45" t="n">
-        <v>61630</v>
+        <v>60240</v>
       </c>
       <c r="B45" t="s">
-        <v>4</v>
+        <v>101</v>
       </c>
       <c r="C45" t="s">
-        <v>4</v>
+        <v>101</v>
       </c>
       <c r="D45" t="n">
-        <v>62.2583</v>
+        <v>62.191</v>
       </c>
       <c r="E45" t="n">
-        <v>8.2</v>
+        <v>6.9933</v>
       </c>
       <c r="F45" t="n">
-        <v>147324</v>
+        <v>84027</v>
       </c>
       <c r="G45" t="n">
-        <v>6921509</v>
+        <v>6921226</v>
       </c>
       <c r="H45" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="I45" t="n">
-        <v>579</v>
+        <v>900</v>
       </c>
     </row>
     <row r="46" spans="1:9">
       <c r="A46" t="n">
-        <v>60190</v>
+        <v>61410</v>
       </c>
       <c r="B46" t="s">
         <v>59</v>
@@ -1937,196 +2003,660 @@
         <v>59</v>
       </c>
       <c r="D46" t="n">
-        <v>62.3065</v>
+        <v>62.4555</v>
       </c>
       <c r="E46" t="n">
-        <v>6.849</v>
+        <v>7.7703</v>
       </c>
       <c r="F46" t="n">
-        <v>78180</v>
+        <v>127561</v>
       </c>
       <c r="G46" t="n">
-        <v>6934957</v>
+        <v>6945799</v>
       </c>
       <c r="H46" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="I46" t="n">
-        <v>1050</v>
+        <v>1294</v>
       </c>
     </row>
     <row r="47" spans="1:9">
       <c r="A47" t="n">
-        <v>25830</v>
+        <v>87772</v>
       </c>
       <c r="B47" t="s">
-        <v>13</v>
+        <v>86</v>
       </c>
       <c r="C47" t="s">
-        <v>13</v>
+        <v>87</v>
       </c>
       <c r="D47" t="n">
-        <v>60.5917</v>
+        <v>68.5863</v>
       </c>
       <c r="E47" t="n">
-        <v>7.5242</v>
+        <v>16.3608</v>
       </c>
       <c r="F47" t="n">
-        <v>91089</v>
+        <v>555442</v>
       </c>
       <c r="G47" t="n">
-        <v>6740599</v>
+        <v>7608847</v>
       </c>
       <c r="H47" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="I47" t="n">
-        <v>1210</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="48" spans="1:9">
       <c r="A48" t="n">
-        <v>61410</v>
+        <v>31250</v>
       </c>
       <c r="B48" t="s">
-        <v>46</v>
+        <v>84</v>
       </c>
       <c r="C48" t="s">
-        <v>46</v>
+        <v>84</v>
       </c>
       <c r="D48" t="n">
-        <v>62.4555</v>
+        <v>59.9953</v>
       </c>
       <c r="E48" t="n">
-        <v>7.7703</v>
+        <v>8.3777</v>
       </c>
       <c r="F48" t="n">
-        <v>127561</v>
+        <v>130983</v>
       </c>
       <c r="G48" t="n">
-        <v>6945799</v>
+        <v>6669386</v>
       </c>
       <c r="H48" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="I48" t="n">
-        <v>1294</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="49" spans="1:9">
       <c r="A49" t="n">
-        <v>64700</v>
+        <v>91729</v>
       </c>
       <c r="B49" t="s">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="C49" t="s">
-        <v>35</v>
+        <v>1</v>
       </c>
       <c r="D49" t="n">
-        <v>62.722</v>
+        <v>70.075</v>
       </c>
       <c r="E49" t="n">
-        <v>8.7753</v>
+        <v>20.431</v>
       </c>
       <c r="F49" t="n">
-        <v>182072</v>
+        <v>706325</v>
       </c>
       <c r="G49" t="n">
-        <v>6969987</v>
+        <v>7783439</v>
       </c>
       <c r="H49" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="I49" t="n">
-        <v>405</v>
+        <v>850</v>
       </c>
     </row>
     <row r="50" spans="1:9">
       <c r="A50" t="n">
-        <v>10800</v>
+        <v>54710</v>
       </c>
       <c r="B50" t="s">
-        <v>69</v>
+        <v>12</v>
       </c>
       <c r="C50" t="s">
-        <v>69</v>
+        <v>13</v>
       </c>
       <c r="D50" t="n">
-        <v>62.6794</v>
+        <v>61.178</v>
       </c>
       <c r="E50" t="n">
-        <v>11.8153</v>
+        <v>8.1125</v>
       </c>
       <c r="F50" t="n">
-        <v>336969</v>
+        <v>130049</v>
       </c>
       <c r="G50" t="n">
-        <v>6953897</v>
+        <v>6802130</v>
       </c>
       <c r="H50" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="I50" t="n">
-        <v>760</v>
+        <v>956</v>
       </c>
     </row>
     <row r="51" spans="1:9">
       <c r="A51" t="n">
-        <v>31620</v>
+        <v>30875</v>
       </c>
       <c r="B51" t="s">
-        <v>52</v>
+        <v>5</v>
       </c>
       <c r="C51" t="s">
-        <v>53</v>
+        <v>5</v>
       </c>
       <c r="D51" t="n">
-        <v>59.8397</v>
+        <v>59.8103</v>
       </c>
       <c r="E51" t="n">
-        <v>8.1792</v>
+        <v>8.9872</v>
       </c>
       <c r="F51" t="n">
-        <v>118161</v>
+        <v>163008</v>
       </c>
       <c r="G51" t="n">
-        <v>6653245</v>
+        <v>6645590</v>
       </c>
       <c r="H51" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="I51" t="n">
-        <v>977</v>
+        <v>240</v>
       </c>
     </row>
     <row r="52" spans="1:9">
       <c r="A52" t="n">
+        <v>25630</v>
+      </c>
+      <c r="B52" t="s">
+        <v>22</v>
+      </c>
+      <c r="C52" t="s">
+        <v>23</v>
+      </c>
+      <c r="D52" t="n">
+        <v>60.53</v>
+      </c>
+      <c r="E52" t="n">
+        <v>8.1948</v>
+      </c>
+      <c r="F52" t="n">
+        <v>126964</v>
+      </c>
+      <c r="G52" t="n">
+        <v>6729759</v>
+      </c>
+      <c r="H52" t="s">
+        <v>96</v>
+      </c>
+      <c r="I52" t="n">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9">
+      <c r="A53" t="n">
+        <v>40880</v>
+      </c>
+      <c r="B53" t="s">
+        <v>39</v>
+      </c>
+      <c r="C53" t="s">
+        <v>40</v>
+      </c>
+      <c r="D53" t="n">
+        <v>59.5766</v>
+      </c>
+      <c r="E53" t="n">
+        <v>7.3897</v>
+      </c>
+      <c r="F53" t="n">
+        <v>70721</v>
+      </c>
+      <c r="G53" t="n">
+        <v>6628898</v>
+      </c>
+      <c r="H53" t="s">
+        <v>96</v>
+      </c>
+      <c r="I53" t="n">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9">
+      <c r="A54" t="n">
+        <v>9380</v>
+      </c>
+      <c r="B54" t="s">
+        <v>82</v>
+      </c>
+      <c r="C54" t="s">
+        <v>82</v>
+      </c>
+      <c r="D54" t="n">
+        <v>62.2958</v>
+      </c>
+      <c r="E54" t="n">
+        <v>9.352</v>
+      </c>
+      <c r="F54" t="n">
+        <v>207315</v>
+      </c>
+      <c r="G54" t="n">
+        <v>6919920</v>
+      </c>
+      <c r="H54" t="s">
+        <v>96</v>
+      </c>
+      <c r="I54" t="n">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9">
+      <c r="A55" t="n">
+        <v>32890</v>
+      </c>
+      <c r="B55" t="s">
+        <v>41</v>
+      </c>
+      <c r="C55" t="s">
+        <v>42</v>
+      </c>
+      <c r="D55" t="n">
+        <v>59.497</v>
+      </c>
+      <c r="E55" t="n">
+        <v>8.1992</v>
+      </c>
+      <c r="F55" t="n">
+        <v>115363</v>
+      </c>
+      <c r="G55" t="n">
+        <v>6615099</v>
+      </c>
+      <c r="H55" t="s">
+        <v>96</v>
+      </c>
+      <c r="I55" t="n">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9">
+      <c r="A56" t="n">
+        <v>89980</v>
+      </c>
+      <c r="B56" t="s">
+        <v>89</v>
+      </c>
+      <c r="C56" t="s">
+        <v>89</v>
+      </c>
+      <c r="D56" t="n">
+        <v>69.0935</v>
+      </c>
+      <c r="E56" t="n">
+        <v>19.6278</v>
+      </c>
+      <c r="F56" t="n">
+        <v>684149</v>
+      </c>
+      <c r="G56" t="n">
+        <v>7671740</v>
+      </c>
+      <c r="H56" t="s">
+        <v>96</v>
+      </c>
+      <c r="I56" t="n">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9">
+      <c r="A57" t="n">
+        <v>31970</v>
+      </c>
+      <c r="B57" t="s">
+        <v>21</v>
+      </c>
+      <c r="C57" t="s">
+        <v>21</v>
+      </c>
+      <c r="D57" t="n">
+        <v>59.8497</v>
+      </c>
+      <c r="E57" t="n">
+        <v>8.6562</v>
+      </c>
+      <c r="F57" t="n">
+        <v>144914</v>
+      </c>
+      <c r="G57" t="n">
+        <v>6651697</v>
+      </c>
+      <c r="H57" t="s">
+        <v>96</v>
+      </c>
+      <c r="I57" t="n">
+        <v>1804</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9">
+      <c r="A58" t="n">
+        <v>89940</v>
+      </c>
+      <c r="B58" t="s">
+        <v>6</v>
+      </c>
+      <c r="C58" t="s">
+        <v>7</v>
+      </c>
+      <c r="D58" t="n">
+        <v>68.7817</v>
+      </c>
+      <c r="E58" t="n">
+        <v>19.7017</v>
+      </c>
+      <c r="F58" t="n">
+        <v>689747</v>
+      </c>
+      <c r="G58" t="n">
+        <v>7637284</v>
+      </c>
+      <c r="H58" t="s">
+        <v>96</v>
+      </c>
+      <c r="I58" t="n">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9">
+      <c r="A59" t="n">
+        <v>59695</v>
+      </c>
+      <c r="B59" t="s">
+        <v>104</v>
+      </c>
+      <c r="C59" t="s">
+        <v>105</v>
+      </c>
+      <c r="D59" t="n">
+        <v>62.16</v>
+      </c>
+      <c r="E59" t="n">
+        <v>6.2877</v>
+      </c>
+      <c r="F59" t="n">
+        <v>47058</v>
+      </c>
+      <c r="G59" t="n">
+        <v>6922540</v>
+      </c>
+      <c r="H59" t="s">
+        <v>96</v>
+      </c>
+      <c r="I59" t="n">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9">
+      <c r="A60" t="n">
         <v>53530</v>
       </c>
-      <c r="B52" t="s">
-        <v>47</v>
-      </c>
-      <c r="C52" t="s">
-        <v>47</v>
-      </c>
-      <c r="D52" t="n">
+      <c r="B60" t="s">
+        <v>60</v>
+      </c>
+      <c r="C60" t="s">
+        <v>60</v>
+      </c>
+      <c r="D60" t="n">
         <v>60.6563</v>
       </c>
-      <c r="E52" t="n">
+      <c r="E60" t="n">
         <v>7.2755</v>
       </c>
-      <c r="F52" t="n">
+      <c r="F60" t="n">
         <v>78375</v>
       </c>
-      <c r="G52" t="n">
+      <c r="G60" t="n">
         <v>6749336</v>
       </c>
-      <c r="H52" t="s">
-        <v>76</v>
-      </c>
-      <c r="I52" t="n">
+      <c r="H60" t="s">
+        <v>96</v>
+      </c>
+      <c r="I60" t="n">
         <v>1162</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9">
+      <c r="A61" t="n">
+        <v>13655</v>
+      </c>
+      <c r="B61" t="s">
+        <v>81</v>
+      </c>
+      <c r="C61" t="s">
+        <v>81</v>
+      </c>
+      <c r="D61" t="n">
+        <v>61.5308</v>
+      </c>
+      <c r="E61" t="n">
+        <v>9.4023</v>
+      </c>
+      <c r="F61" t="n">
+        <v>202568</v>
+      </c>
+      <c r="G61" t="n">
+        <v>6834700</v>
+      </c>
+      <c r="H61" t="s">
+        <v>96</v>
+      </c>
+      <c r="I61" t="n">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9">
+      <c r="A62" t="n">
+        <v>31620</v>
+      </c>
+      <c r="B62" t="s">
+        <v>67</v>
+      </c>
+      <c r="C62" t="s">
+        <v>68</v>
+      </c>
+      <c r="D62" t="n">
+        <v>59.8397</v>
+      </c>
+      <c r="E62" t="n">
+        <v>8.1792</v>
+      </c>
+      <c r="F62" t="n">
+        <v>118161</v>
+      </c>
+      <c r="G62" t="n">
+        <v>6653245</v>
+      </c>
+      <c r="H62" t="s">
+        <v>96</v>
+      </c>
+      <c r="I62" t="n">
+        <v>977</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9">
+      <c r="A63" t="n">
+        <v>89985</v>
+      </c>
+      <c r="B63" t="s">
+        <v>80</v>
+      </c>
+      <c r="C63" t="s">
+        <v>80</v>
+      </c>
+      <c r="D63" t="n">
+        <v>69.1025</v>
+      </c>
+      <c r="E63" t="n">
+        <v>19.5442</v>
+      </c>
+      <c r="F63" t="n">
+        <v>680754</v>
+      </c>
+      <c r="G63" t="n">
+        <v>7672492</v>
+      </c>
+      <c r="H63" t="s">
+        <v>96</v>
+      </c>
+      <c r="I63" t="n">
+        <v>1020</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9">
+      <c r="A64" t="n">
+        <v>53160</v>
+      </c>
+      <c r="B64" t="s">
+        <v>44</v>
+      </c>
+      <c r="C64" t="s">
+        <v>45</v>
+      </c>
+      <c r="D64" t="n">
+        <v>60.9004</v>
+      </c>
+      <c r="E64" t="n">
+        <v>6.7243</v>
+      </c>
+      <c r="F64" t="n">
+        <v>51827</v>
+      </c>
+      <c r="G64" t="n">
+        <v>6780047</v>
+      </c>
+      <c r="H64" t="s">
+        <v>96</v>
+      </c>
+      <c r="I64" t="n">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9">
+      <c r="A65" t="n">
+        <v>91120</v>
+      </c>
+      <c r="B65" t="s">
+        <v>54</v>
+      </c>
+      <c r="C65" t="s">
+        <v>55</v>
+      </c>
+      <c r="D65" t="n">
+        <v>69.5592</v>
+      </c>
+      <c r="E65" t="n">
+        <v>20.1502</v>
+      </c>
+      <c r="F65" t="n">
+        <v>700531</v>
+      </c>
+      <c r="G65" t="n">
+        <v>7725170</v>
+      </c>
+      <c r="H65" t="s">
+        <v>96</v>
+      </c>
+      <c r="I65" t="n">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9">
+      <c r="A66" t="n">
+        <v>42940</v>
+      </c>
+      <c r="B66" t="s">
+        <v>78</v>
+      </c>
+      <c r="C66" t="s">
+        <v>79</v>
+      </c>
+      <c r="D66" t="n">
+        <v>58.923</v>
+      </c>
+      <c r="E66" t="n">
+        <v>6.9097</v>
+      </c>
+      <c r="F66" t="n">
+        <v>34883</v>
+      </c>
+      <c r="G66" t="n">
+        <v>6559675</v>
+      </c>
+      <c r="H66" t="s">
+        <v>96</v>
+      </c>
+      <c r="I66" t="n">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9">
+      <c r="A67" t="n">
+        <v>90400</v>
+      </c>
+      <c r="B67" t="s">
+        <v>91</v>
+      </c>
+      <c r="C67" t="s">
+        <v>92</v>
+      </c>
+      <c r="D67" t="n">
+        <v>69.6523</v>
+      </c>
+      <c r="E67" t="n">
+        <v>18.9057</v>
+      </c>
+      <c r="F67" t="n">
+        <v>651477</v>
+      </c>
+      <c r="G67" t="n">
+        <v>7731942</v>
+      </c>
+      <c r="H67" t="s">
+        <v>96</v>
+      </c>
+      <c r="I67" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9">
+      <c r="A68" t="n">
+        <v>80705</v>
+      </c>
+      <c r="B68" t="s">
+        <v>24</v>
+      </c>
+      <c r="C68" t="s">
+        <v>25</v>
+      </c>
+      <c r="D68" t="n">
+        <v>66.8275</v>
+      </c>
+      <c r="E68" t="n">
+        <v>13.948</v>
+      </c>
+      <c r="F68" t="n">
+        <v>453807</v>
+      </c>
+      <c r="G68" t="n">
+        <v>7412540</v>
+      </c>
+      <c r="H68" t="s">
+        <v>96</v>
+      </c>
+      <c r="I68" t="n">
+        <v>520</v>
       </c>
     </row>
   </sheetData>

</xml_diff>